<commit_message>
Fixing execution from maven
</commit_message>
<xml_diff>
--- a/TestExecutor/src/main/resources/testData.xlsx
+++ b/TestExecutor/src/main/resources/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Enquero_Automation_Framework\TestExecutor\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B941E042-383F-4E6D-B68B-0FE715E95915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0116FB-2F8A-4DBA-A2C0-8D9C869A0361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03C0641D-4EAF-4ECB-AF6B-6704CD8ABCFB}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>ValidationParameters</t>
   </si>
   <si>
-    <t>{textToValidate:Welcome Vivek!!}</t>
-  </si>
-  <si>
-    <t>{textToValidate:Order Create Successfully}</t>
-  </si>
-  <si>
     <t>testLoginFacebook</t>
   </si>
   <si>
@@ -59,16 +53,22 @@
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>{username:SwatiChetty,password:123456}</t>
-  </si>
-  <si>
-    <t>{username:Swati,password:123}</t>
-  </si>
-  <si>
     <t>tc1</t>
   </si>
   <si>
     <t>tc2</t>
+  </si>
+  <si>
+    <t>{"username":"SwatiChetty","password":"123456"}</t>
+  </si>
+  <si>
+    <t>{"textToValidate":"Welcome Vivek!!"}</t>
+  </si>
+  <si>
+    <t>{"username":"Swati","password":"123"}</t>
+  </si>
+  <si>
+    <t>{"textToValidate":"Order Create Successfully"}</t>
   </si>
 </sst>
 </file>
@@ -423,22 +423,23 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.1796875" customWidth="1"/>
     <col min="2" max="2" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.453125" customWidth="1"/>
+    <col min="4" max="4" width="36.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -449,7 +450,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -458,21 +459,21 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -481,12 +482,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -693,15 +691,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{521A633E-B03D-4D65-9917-E953736D8D12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C234376-B86F-4B81-801E-F3A2527A814A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8ea24074-1ae4-4d8a-bed5-50beddb226f9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1dfacc6d-6701-4530-a587-2da6e9f4a883"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -726,18 +736,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C234376-B86F-4B81-801E-F3A2527A814A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{521A633E-B03D-4D65-9917-E953736D8D12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8ea24074-1ae4-4d8a-bed5-50beddb226f9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1dfacc6d-6701-4530-a587-2da6e9f4a883"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>